<commit_message>
First commit - upload dashboard and data files
</commit_message>
<xml_diff>
--- a/data/2008 IP MASTERLIST.xlsx
+++ b/data/2008 IP MASTERLIST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ip_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8149638-6F72-4DE6-815E-5F87906480DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381BA411-5FA7-45B2-BE64-D2A69F435C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
   <si>
     <t>IPRO file number</t>
   </si>
@@ -309,15 +309,9 @@
     <t>978-971-006-000-9</t>
   </si>
   <si>
-    <t>Starting Date/ Frequency</t>
-  </si>
-  <si>
     <t>2008-Br.1-01</t>
   </si>
   <si>
-    <t>March 2008, Annually</t>
-  </si>
-  <si>
     <t>2012-0192</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>CEAT R&amp;E Journal</t>
   </si>
   <si>
-    <t>November 1, 2008, Quarterly</t>
-  </si>
-  <si>
     <t>2012-032X</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>Proceedings 2008, Agency In-House Review</t>
   </si>
   <si>
-    <t>2008, Annually</t>
-  </si>
-  <si>
     <t>2012-2829</t>
   </si>
   <si>
@@ -352,6 +340,21 @@
   </si>
   <si>
     <t>Others: IECs, Non Research Technoguides, Journals</t>
+  </si>
+  <si>
+    <t>Starting Date</t>
+  </si>
+  <si>
+    <t>Annualy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarterly </t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>Frequency</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -442,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,26 +471,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,8 +719,8 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
@@ -1150,7 +1160,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>78</v>
@@ -1180,7 +1190,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>79</v>
@@ -1209,7 +1219,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>79</v>
@@ -1238,7 +1248,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>79</v>
@@ -1294,11 +1304,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S127"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1311,18 +1321,14 @@
     <col min="7" max="7" width="12.6640625" style="17"/>
     <col min="8" max="8" width="18.77734375" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="17"/>
-    <col min="12" max="12" width="62.109375" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="17"/>
-    <col min="18" max="18" width="21.6640625" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
@@ -1345,35 +1351,8 @@
       <c r="I1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1399,33 +1378,8 @@
       <c r="I2" s="16">
         <v>39518</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="24">
-        <v>39518</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="S2" s="19">
-        <v>39518</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>85</v>
       </c>
@@ -1451,89 +1405,117 @@
       <c r="I3" s="23">
         <v>39700</v>
       </c>
-      <c r="K3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="24">
+        <v>39518</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="19">
+        <v>39518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="B5" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="11" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="G5" s="20">
         <v>39700</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="S3" s="20">
+      <c r="I5" s="20">
         <v>39700</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="K4" s="9" t="s">
+    <row r="6" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="G6" s="20">
         <v>39700</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="20">
+      <c r="I6" s="20">
         <v>39700</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
     </row>
-    <row r="8" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="21"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="21"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="21"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="21"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="21"/>
@@ -1543,7 +1525,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="21"/>
@@ -1553,7 +1535,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="21"/>
@@ -1563,7 +1545,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="21"/>
@@ -1573,7 +1555,7 @@
       <c r="G15" s="21"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="21"/>
@@ -1854,14 +1836,14 @@
       <c r="G53" s="21"/>
     </row>
     <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C55" s="21"/>
@@ -2084,14 +2066,14 @@
       <c r="E97" s="12"/>
     </row>
     <row r="98" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="30"/>
+      <c r="F98" s="30"/>
+      <c r="G98" s="30"/>
+      <c r="H98" s="30"/>
     </row>
     <row r="99" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C99" s="21"/>
@@ -2232,11 +2214,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2244,17 +2226,18 @@
     <col min="1" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="16" style="17" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="17"/>
-    <col min="9" max="9" width="12.6640625" style="17"/>
+    <col min="5" max="5" width="23.6640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="17"/>
+    <col min="10" max="10" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
@@ -2263,24 +2246,27 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>77</v>
@@ -2289,714 +2275,830 @@
       <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="27">
+        <v>39508</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="16">
+        <v>39518</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="16">
+        <v>39518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="16">
-        <v>39518</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="16">
-        <v>39518</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="28">
+        <v>39753</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="16">
+        <v>39546</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="16">
+        <v>39546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="16">
-        <v>39546</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="16">
-        <v>39546</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2008</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="23">
+      <c r="H4" s="23">
         <v>39700</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="23">
+      <c r="I4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="23">
         <v>39700</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C5" s="21"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C6" s="21"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C7" s="21"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C8" s="21"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C12" s="21"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F12" s="12"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C13" s="21"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F13" s="12"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C14" s="21"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F14" s="12"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C15" s="21"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="25"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E15" s="12"/>
+      <c r="F15" s="25"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C16" s="21"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="G16" s="21"/>
-    </row>
-    <row r="17" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F16" s="12"/>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C17" s="21"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F17" s="12"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C18" s="21"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="G18" s="21"/>
-    </row>
-    <row r="19" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F18" s="12"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C19" s="21"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F19" s="12"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C20" s="21"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F20" s="12"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C21" s="21"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F21" s="12"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C22" s="21"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F22" s="12"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C23" s="21"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F23" s="12"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C24" s="21"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C25" s="21"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C26" s="21"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C27" s="21"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C28" s="21"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C29" s="21"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C30" s="21"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C31" s="21"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C32" s="21"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C33" s="21"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C34" s="21"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F34" s="12"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C35" s="21"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F35" s="12"/>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C36" s="21"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
-      <c r="G36" s="22"/>
-    </row>
-    <row r="37" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C37" s="21"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
-      <c r="G37" s="21"/>
-    </row>
-    <row r="38" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F37" s="12"/>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C38" s="21"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
-      <c r="G38" s="21"/>
-    </row>
-    <row r="39" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F38" s="12"/>
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C39" s="21"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
-      <c r="G39" s="21"/>
-    </row>
-    <row r="40" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F39" s="12"/>
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C40" s="21"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
-      <c r="G40" s="21"/>
-    </row>
-    <row r="41" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F40" s="12"/>
+      <c r="H40" s="21"/>
+    </row>
+    <row r="41" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C41" s="21"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F41" s="12"/>
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C42" s="21"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
-      <c r="G42" s="21"/>
-    </row>
-    <row r="43" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F42" s="12"/>
+      <c r="H42" s="21"/>
+    </row>
+    <row r="43" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C43" s="21"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
-      <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F43" s="12"/>
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C44" s="21"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
-      <c r="G44" s="21"/>
-    </row>
-    <row r="45" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F44" s="12"/>
+      <c r="H44" s="21"/>
+    </row>
+    <row r="45" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C45" s="21"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
-      <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F45" s="12"/>
+      <c r="H45" s="21"/>
+    </row>
+    <row r="46" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C46" s="21"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F46" s="12"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C47" s="21"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
-      <c r="G47" s="21"/>
-    </row>
-    <row r="48" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F47" s="12"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C48" s="21"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
-      <c r="G48" s="21"/>
-    </row>
-    <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F48" s="12"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C49" s="21"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
-      <c r="G49" s="21"/>
-    </row>
-    <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F49" s="12"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C50" s="21"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
-      <c r="G50" s="21"/>
-    </row>
-    <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F50" s="12"/>
+      <c r="H50" s="21"/>
+    </row>
+    <row r="51" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C51" s="21"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
-      <c r="G51" s="21"/>
-    </row>
-    <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F51" s="12"/>
+      <c r="H51" s="21"/>
+    </row>
+    <row r="52" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C52" s="21"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
-      <c r="G52" s="21"/>
-    </row>
-    <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F52" s="12"/>
+      <c r="H52" s="21"/>
+    </row>
+    <row r="53" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C53" s="21"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
-      <c r="G53" s="21"/>
-    </row>
-    <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F53" s="12"/>
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C54" s="21"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
-      <c r="G54" s="21"/>
-    </row>
-    <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="27"/>
-    </row>
-    <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F54" s="12"/>
+      <c r="H54" s="21"/>
+    </row>
+    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="30"/>
+    </row>
+    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C56" s="21"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
-      <c r="G56" s="21"/>
-    </row>
-    <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F56" s="12"/>
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C57" s="21"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
-      <c r="G57" s="21"/>
-    </row>
-    <row r="58" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F57" s="12"/>
+      <c r="H57" s="21"/>
+    </row>
+    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C58" s="21"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
-      <c r="G58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F58" s="12"/>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C59" s="21"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
-      <c r="G59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F59" s="12"/>
+      <c r="H59" s="21"/>
+    </row>
+    <row r="60" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C60" s="21"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
-      <c r="G60" s="21"/>
-    </row>
-    <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F60" s="12"/>
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C61" s="21"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
-      <c r="G61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F61" s="12"/>
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C62" s="21"/>
       <c r="D62" s="12"/>
-    </row>
-    <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E62" s="12"/>
+    </row>
+    <row r="63" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C63" s="21"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
-    </row>
-    <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C64" s="21"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
-    </row>
-    <row r="65" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C65" s="21"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
-    </row>
-    <row r="66" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C66" s="21"/>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C67" s="21"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
-    </row>
-    <row r="68" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C68" s="21"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
-    </row>
-    <row r="69" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C69" s="21"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
-    </row>
-    <row r="70" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C70" s="21"/>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
-    </row>
-    <row r="71" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C71" s="21"/>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
-    </row>
-    <row r="72" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C72" s="21"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
-    </row>
-    <row r="73" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F72" s="12"/>
+    </row>
+    <row r="73" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C73" s="21"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
-    </row>
-    <row r="74" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C74" s="21"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
-    </row>
-    <row r="75" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F74" s="12"/>
+    </row>
+    <row r="75" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C75" s="21"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
-    </row>
-    <row r="76" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C76" s="21"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
-    </row>
-    <row r="77" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C77" s="21"/>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
-    </row>
-    <row r="78" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C78" s="21"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
-    </row>
-    <row r="79" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C79" s="21"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
-    </row>
-    <row r="80" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C80" s="21"/>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
-    </row>
-    <row r="81" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C81" s="21"/>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
-    </row>
-    <row r="82" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F81" s="12"/>
+    </row>
+    <row r="82" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C82" s="21"/>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F82" s="12"/>
+    </row>
+    <row r="83" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C83" s="21"/>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
-    </row>
-    <row r="84" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C84" s="21"/>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
-    </row>
-    <row r="85" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F84" s="12"/>
+    </row>
+    <row r="85" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C85" s="21"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
-    </row>
-    <row r="86" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F85" s="12"/>
+    </row>
+    <row r="86" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C86" s="21"/>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F86" s="12"/>
+    </row>
+    <row r="87" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C87" s="21"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
-    </row>
-    <row r="88" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F87" s="12"/>
+    </row>
+    <row r="88" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C88" s="21"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
-    </row>
-    <row r="89" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F88" s="12"/>
+    </row>
+    <row r="89" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C89" s="21"/>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
-    </row>
-    <row r="90" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F89" s="12"/>
+    </row>
+    <row r="90" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C90" s="21"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
-    </row>
-    <row r="91" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F90" s="12"/>
+    </row>
+    <row r="91" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C91" s="21"/>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
-    </row>
-    <row r="92" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F91" s="12"/>
+    </row>
+    <row r="92" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C92" s="21"/>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
-    </row>
-    <row r="93" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F92" s="12"/>
+    </row>
+    <row r="93" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C93" s="21"/>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
-    </row>
-    <row r="94" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F93" s="12"/>
+    </row>
+    <row r="94" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C94" s="21"/>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
-    </row>
-    <row r="95" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F94" s="12"/>
+    </row>
+    <row r="95" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C95" s="21"/>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
-    </row>
-    <row r="96" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F95" s="12"/>
+    </row>
+    <row r="96" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C96" s="21"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
-    </row>
-    <row r="97" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F96" s="12"/>
+    </row>
+    <row r="97" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C97" s="21"/>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
-    </row>
-    <row r="98" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F97" s="12"/>
+    </row>
+    <row r="98" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C98" s="21"/>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
-    </row>
-    <row r="99" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="27"/>
-    </row>
-    <row r="100" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F98" s="12"/>
+    </row>
+    <row r="99" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="31"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
+      <c r="G99" s="30"/>
+      <c r="H99" s="31"/>
+      <c r="I99" s="30"/>
+    </row>
+    <row r="100" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C100" s="21"/>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
-    </row>
-    <row r="101" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F100" s="12"/>
+    </row>
+    <row r="101" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C101" s="21"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
-    </row>
-    <row r="102" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F101" s="12"/>
+    </row>
+    <row r="102" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C102" s="21"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
-    </row>
-    <row r="103" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F102" s="12"/>
+    </row>
+    <row r="103" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C103" s="21"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
-    </row>
-    <row r="104" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F103" s="12"/>
+    </row>
+    <row r="104" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C104" s="21"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
-    </row>
-    <row r="105" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F104" s="12"/>
+    </row>
+    <row r="105" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C105" s="21"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
-    </row>
-    <row r="106" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F105" s="12"/>
+    </row>
+    <row r="106" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C106" s="21"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
-    </row>
-    <row r="107" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F106" s="12"/>
+    </row>
+    <row r="107" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C107" s="21"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
-    </row>
-    <row r="108" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F107" s="12"/>
+    </row>
+    <row r="108" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C108" s="21"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
-    </row>
-    <row r="109" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F108" s="12"/>
+    </row>
+    <row r="109" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C109" s="21"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
-    </row>
-    <row r="110" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F109" s="12"/>
+    </row>
+    <row r="110" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C110" s="21"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
-    </row>
-    <row r="111" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F110" s="12"/>
+    </row>
+    <row r="111" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C111" s="21"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
-    </row>
-    <row r="112" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F111" s="12"/>
+    </row>
+    <row r="112" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C112" s="21"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
-    </row>
-    <row r="113" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F112" s="12"/>
+    </row>
+    <row r="113" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C113" s="21"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
-    </row>
-    <row r="114" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F113" s="12"/>
+    </row>
+    <row r="114" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C114" s="21"/>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
-    </row>
-    <row r="115" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F114" s="12"/>
+    </row>
+    <row r="115" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C115" s="21"/>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
-    </row>
-    <row r="116" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F115" s="12"/>
+    </row>
+    <row r="116" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C116" s="21"/>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
-    </row>
-    <row r="117" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F116" s="12"/>
+    </row>
+    <row r="117" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C117" s="21"/>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
-    </row>
-    <row r="118" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F117" s="12"/>
+    </row>
+    <row r="118" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C118" s="21"/>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
-    </row>
-    <row r="119" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F118" s="12"/>
+    </row>
+    <row r="119" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C119" s="21"/>
     </row>
-    <row r="120" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C120" s="21"/>
     </row>
-    <row r="121" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C121" s="21"/>
     </row>
-    <row r="122" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C122" s="21"/>
     </row>
-    <row r="123" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C123" s="21"/>
     </row>
-    <row r="124" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C124" s="21"/>
     </row>
-    <row r="125" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C125" s="21"/>
     </row>
-    <row r="126" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C126" s="21"/>
     </row>
-    <row r="127" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C127" s="21"/>
     </row>
-    <row r="128" spans="3:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C128" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A99:H99"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A99:I99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>